<commit_message>
Fixed the other issues
</commit_message>
<xml_diff>
--- a/timetable.xlsx
+++ b/timetable.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="13">
   <si>
     <t xml:space="preserve">Class</t>
   </si>
@@ -343,7 +343,7 @@
   <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
+      <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -426,70 +426,34 @@
       </c>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>5</v>
-      </c>
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>7</v>
-      </c>
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>9</v>
-      </c>
+      <c r="A10" s="1"/>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>11</v>
-      </c>
+      <c r="A11" s="1"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>12</v>
-      </c>
+      <c r="A12" s="1"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
     </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>9</v>
-      </c>
+      <c r="A13" s="1"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
trying to improve the layout for printing A4 size paper.
</commit_message>
<xml_diff>
--- a/timetable.xlsx
+++ b/timetable.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="13">
   <si>
     <t xml:space="preserve">Class</t>
   </si>
@@ -343,7 +343,7 @@
   <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
+      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8:C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -426,34 +426,70 @@
       </c>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1"/>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
+      <c r="A8" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="1"/>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
+      <c r="A9" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
+      <c r="A10" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="1"/>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
+      <c r="A11" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="1"/>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
+      <c r="A12" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="1"/>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
+      <c r="A13" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>9</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
Address Field added and modified a little bit
</commit_message>
<xml_diff>
--- a/timetable.xlsx
+++ b/timetable.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="27">
   <si>
     <t xml:space="preserve">Class</t>
   </si>
@@ -31,34 +31,76 @@
     <t xml:space="preserve">Subject</t>
   </si>
   <si>
-    <t xml:space="preserve">10A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">25-10-2025</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mathematics</t>
-  </si>
-  <si>
-    <t xml:space="preserve">28-10-2025</t>
+    <t xml:space="preserve">Nursery</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11-10-2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Maths (w)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">13-10-2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hindi (w)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">14-10-2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">English (w)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">15-10-2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Maths (oral) , GK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">16-10-2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hindi Poem (oral) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">17-10-2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">English Rhymes (oral)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LKG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UKG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hindi </t>
   </si>
   <si>
     <t xml:space="preserve">Science</t>
   </si>
   <si>
-    <t xml:space="preserve">30-10-2025</t>
-  </si>
-  <si>
-    <t xml:space="preserve">English</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10B</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Social Science</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Computer</t>
+    <t xml:space="preserve">English </t>
+  </si>
+  <si>
+    <t xml:space="preserve">MSC / GK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Maths</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Oral</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EVS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sanskrit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SST</t>
   </si>
 </sst>
 </file>
@@ -340,13 +382,16 @@
     <outlinePr summaryBelow="0"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8:C13"/>
+      <selection pane="topLeft" activeCell="D53" activeCellId="0" sqref="D53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="23.33"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -360,137 +405,666 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="0" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="0" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="0" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="0" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="0" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" s="0" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" s="0" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="s">
-        <v>10</v>
+      <c r="A6" s="0" t="s">
+        <v>3</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C6" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="s">
-        <v>10</v>
+      <c r="C6" s="0" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>3</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>9</v>
+        <v>14</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1" t="s">
-        <v>3</v>
+      <c r="A8" s="0" t="s">
+        <v>16</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C8" s="0" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="1" t="s">
-        <v>3</v>
+      <c r="A9" s="0" t="s">
+        <v>16</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C9" s="0" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="1" t="s">
-        <v>3</v>
+      <c r="A10" s="0" t="s">
+        <v>16</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C10" s="0" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="1" t="s">
+      <c r="A11" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C11" s="1" t="s">
+      <c r="C11" s="0" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="1" t="s">
+      <c r="A12" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C12" s="0" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13" s="0" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C14" s="0" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C15" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C16" s="0" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="B17" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C12" s="1" t="s">
+      <c r="C17" s="0" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="B18" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="1" t="s">
+      <c r="C18" s="0" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C19" s="0" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C20" s="0" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C21" s="0" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C22" s="0" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B23" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="C23" s="0" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C24" s="0" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C25" s="0" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C26" s="0" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C27" s="0" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="B28" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C13" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
+      <c r="C28" s="0" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A29" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C29" s="0" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A30" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C30" s="0" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A31" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C31" s="0" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A32" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C32" s="0" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A33" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C33" s="0" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A34" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C34" s="0" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A35" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C35" s="0" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A36" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C36" s="0" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A37" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C37" s="0" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A38" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C38" s="0" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A39" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C39" s="0" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A40" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C40" s="0" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A41" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C41" s="0" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A42" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C42" s="0" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A43" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C43" s="0" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A44" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C44" s="0" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A45" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C45" s="0" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A46" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C46" s="0" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A47" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C47" s="0" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A48" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C48" s="0" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A49" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C49" s="0" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A50" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C50" s="0" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A51" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C51" s="0" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A52" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C52" s="0" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A53" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C53" s="0" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A54" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C54" s="0" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A55" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C55" s="0" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A56" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C56" s="0" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A57" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C57" s="0" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A58" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C58" s="0" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A59" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C59" s="0" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A60" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C60" s="0" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A61" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C61" s="0" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>